<commit_message>
Added windows support for parallel processing
</commit_message>
<xml_diff>
--- a/docs/mock_experiment_results.xlsx
+++ b/docs/mock_experiment_results.xlsx
@@ -48,42 +48,42 @@
     <t xml:space="preserve">Column</t>
   </si>
   <si>
+    <t xml:space="preserve">G3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G8</t>
+  </si>
+  <si>
     <t xml:space="preserve">G9</t>
   </si>
   <si>
-    <t xml:space="preserve">cond1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G8</t>
+    <t xml:space="preserve">G2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empty</t>
   </si>
   <si>
     <t xml:space="preserve">G1</t>
   </si>
   <si>
-    <t xml:space="preserve">G7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G6</t>
-  </si>
-  <si>
     <t xml:space="preserve">G4</t>
   </si>
   <si>
-    <t xml:space="preserve">Empty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G3</t>
-  </si>
-  <si>
     <t xml:space="preserve">cond2</t>
   </si>
   <si>
@@ -147,337 +147,337 @@
     <t xml:space="preserve">3</t>
   </si>
   <si>
+    <t xml:space="preserve">cond1_G3_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G2_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G10_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G8_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G7_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G5_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G9_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G6_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G4_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G5_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G5_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G9_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G8_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G6_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G5_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G8_4</t>
+  </si>
+  <si>
     <t xml:space="preserve">cond1_G9_1</t>
   </si>
   <si>
-    <t xml:space="preserve">cond1_G7_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G6_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G8_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G2_3</t>
+    <t xml:space="preserve">cond1_G4_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G10_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G3_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G6_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G5_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G4_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G8_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G7_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G8_3</t>
   </si>
   <si>
     <t xml:space="preserve">cond1_G4_4</t>
   </si>
   <si>
-    <t xml:space="preserve">cond1_G1_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G5_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G2_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G6_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G4_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G8_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G5_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G1_1</t>
+    <t xml:space="preserve">cond1_G10_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond1_G2_1</t>
   </si>
   <si>
     <t xml:space="preserve">cond1_G9_3</t>
   </si>
   <si>
-    <t xml:space="preserve">cond1_G10_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G8_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G9_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G10_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G4_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G5_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G6_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G7_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G3_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G4_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G8_4</t>
-  </si>
-  <si>
     <t xml:space="preserve">cond1_G5_4</t>
   </si>
   <si>
-    <t xml:space="preserve">cond1_G2_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G5_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G10_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G3_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G2_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G9_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G8_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond1_G5_6</t>
+    <t xml:space="preserve">cond2_G9_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G5_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G5_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G8_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G3_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G7_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G4_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G8_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G4_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G1_1</t>
   </si>
   <si>
     <t xml:space="preserve">cond2_G5_5</t>
   </si>
   <si>
+    <t xml:space="preserve">cond2_G2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G9_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G6_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G10_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G8_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G5_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G10_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G4_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">cond2_G2_2</t>
   </si>
   <si>
+    <t xml:space="preserve">cond2_G1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G6_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G9_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G6_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G4_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G8_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G7_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G2_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G5_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G3_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G9_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G5_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond2_G8_5</t>
+  </si>
+  <si>
     <t xml:space="preserve">cond2_G10_1</t>
   </si>
   <si>
-    <t xml:space="preserve">cond2_G9_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G3_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G1_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G4_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G8_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G8_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G5_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G9_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G7_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G2_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G6_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G10_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G4_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G4_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G7_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G2_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G8_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G10_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G6_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G9_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G5_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G5_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G9_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G4_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G8_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G5_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G2_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G8_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G5_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G3_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G1_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond2_G6_1</t>
+    <t xml:space="preserve">cond3_G6_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G7_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G8_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G3_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G9_1</t>
   </si>
   <si>
     <t xml:space="preserve">cond3_G5_3</t>
   </si>
   <si>
+    <t xml:space="preserve">cond3_G2_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G6_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G5_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G9_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G8_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G4_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">cond3_G3_1</t>
   </si>
   <si>
-    <t xml:space="preserve">cond3_G2_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G4_1</t>
+    <t xml:space="preserve">cond3_G5_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G4_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G10_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G9_4</t>
   </si>
   <si>
     <t xml:space="preserve">cond3_G8_1</t>
   </si>
   <si>
-    <t xml:space="preserve">cond3_G1_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G9_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G10_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G5_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G6_2</t>
+    <t xml:space="preserve">cond3_G2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G7_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G5_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G5_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G6_1</t>
   </si>
   <si>
     <t xml:space="preserve">cond3_G10_1</t>
   </si>
   <si>
+    <t xml:space="preserve">cond3_G4_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G8_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G9_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">cond3_G1_3</t>
   </si>
   <si>
-    <t xml:space="preserve">cond3_G2_2</t>
+    <t xml:space="preserve">cond3_G10_2</t>
   </si>
   <si>
     <t xml:space="preserve">cond3_G8_4</t>
   </si>
   <si>
-    <t xml:space="preserve">cond3_G7_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G9_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G5_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G7_1</t>
+    <t xml:space="preserve">cond3_G5_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cond3_G2_3</t>
   </si>
   <si>
     <t xml:space="preserve">cond3_G4_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G6_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G8_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G5_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G2_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G4_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G2_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G6_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G9_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G3_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G5_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G8_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G9_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G5_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G2_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G8_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G10_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G4_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cond3_G1_2</t>
   </si>
 </sst>
 </file>
@@ -877,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -897,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -917,7 +917,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -937,7 +937,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -957,7 +957,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
@@ -977,7 +977,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -1007,13 +1007,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
         <v>2</v>
@@ -1027,13 +1027,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>2</v>
@@ -1047,13 +1047,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>2</v>
@@ -1067,13 +1067,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
         <v>2</v>
@@ -1087,13 +1087,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" t="n">
         <v>2</v>
@@ -1107,13 +1107,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" t="n">
         <v>2</v>
@@ -1133,7 +1133,7 @@
         <v>7</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
         <v>2</v>
@@ -1146,15 +1146,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
+      <c r="A18"/>
       <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C18"/>
       <c r="D18" t="n">
         <v>2</v>
       </c>
@@ -1183,7 +1179,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -1203,13 +1199,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
         <v>3</v>
@@ -1223,13 +1219,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
         <v>3</v>
@@ -1243,7 +1239,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -1263,13 +1259,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" t="n">
         <v>3</v>
@@ -1289,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25" t="n">
         <v>3</v>
@@ -1322,11 +1318,15 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27"/>
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
       <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27"/>
+        <v>7</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
       <c r="D27" t="n">
         <v>3</v>
       </c>
@@ -1355,13 +1355,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
         <v>4</v>
@@ -1375,13 +1375,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
         <v>4</v>
@@ -1395,13 +1395,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
         <v>4</v>
@@ -1415,13 +1415,13 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
         <v>4</v>
@@ -1435,13 +1435,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D33" t="n">
         <v>4</v>
@@ -1455,13 +1455,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
         <v>4</v>
@@ -1475,13 +1475,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" t="n">
         <v>4</v>
@@ -1494,11 +1494,15 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36"/>
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
       <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36"/>
+        <v>7</v>
+      </c>
+      <c r="C36" t="n">
+        <v>3</v>
+      </c>
       <c r="D36" t="n">
         <v>4</v>
       </c>
@@ -1527,13 +1531,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
       <c r="C38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" t="n">
         <v>5</v>
@@ -1547,13 +1551,13 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D39" t="n">
         <v>5</v>
@@ -1567,13 +1571,13 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D40" t="n">
         <v>5</v>
@@ -1587,13 +1591,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D41" t="n">
         <v>5</v>
@@ -1607,13 +1611,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" t="n">
         <v>5</v>
@@ -1627,13 +1631,13 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
       <c r="C43" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D43" t="n">
         <v>5</v>
@@ -1646,15 +1650,11 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
-        <v>17</v>
-      </c>
+      <c r="A44"/>
       <c r="B44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" t="n">
-        <v>2</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C44"/>
       <c r="D44" t="n">
         <v>5</v>
       </c>
@@ -1699,13 +1699,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
         <v>18</v>
       </c>
       <c r="C47" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D47" t="n">
         <v>6</v>
@@ -1719,13 +1719,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
       </c>
       <c r="C48" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D48" t="n">
         <v>6</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
@@ -1759,13 +1759,13 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
         <v>18</v>
       </c>
       <c r="C50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" t="n">
         <v>6</v>
@@ -1779,13 +1779,13 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D51" t="n">
         <v>6</v>
@@ -1799,13 +1799,13 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
         <v>18</v>
       </c>
       <c r="C52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D52" t="n">
         <v>6</v>
@@ -1819,13 +1819,13 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
         <v>18</v>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D53" t="n">
         <v>6</v>
@@ -1839,13 +1839,13 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
       </c>
       <c r="C54" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D54" t="n">
         <v>6</v>
@@ -1881,7 +1881,7 @@
         <v>18</v>
       </c>
       <c r="C56" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D56" t="n">
         <v>7</v>
@@ -1895,13 +1895,13 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
       <c r="C57" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D57" t="n">
         <v>7</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -1935,13 +1935,13 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
         <v>18</v>
       </c>
       <c r="C59" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="n">
         <v>7</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
         <v>18</v>
@@ -1975,13 +1975,13 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
         <v>18</v>
       </c>
       <c r="C61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D61" t="n">
         <v>7</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
         <v>18</v>
@@ -2015,7 +2015,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B63" t="s">
         <v>18</v>
@@ -2051,13 +2051,13 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
         <v>18</v>
       </c>
       <c r="C65" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D65" t="n">
         <v>8</v>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
         <v>18</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
         <v>18</v>
@@ -2111,13 +2111,13 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B68" t="s">
         <v>18</v>
       </c>
       <c r="C68" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D68" t="n">
         <v>8</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B69" t="s">
         <v>18</v>
@@ -2171,13 +2171,13 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
         <v>18</v>
       </c>
       <c r="C71" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D71" t="n">
         <v>8</v>
@@ -2190,15 +2190,11 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="s">
-        <v>13</v>
-      </c>
+      <c r="A72"/>
       <c r="B72" t="s">
-        <v>18</v>
-      </c>
-      <c r="C72" t="n">
-        <v>2</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C72"/>
       <c r="D72" t="n">
         <v>8</v>
       </c>
@@ -2227,7 +2223,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B74" t="s">
         <v>18</v>
@@ -2267,13 +2263,13 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
         <v>18</v>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76" t="n">
         <v>9</v>
@@ -2287,13 +2283,13 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
         <v>18</v>
       </c>
       <c r="C77" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D77" t="n">
         <v>9</v>
@@ -2327,13 +2323,13 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B79" t="s">
         <v>18</v>
       </c>
       <c r="C79" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D79" t="n">
         <v>9</v>
@@ -2347,7 +2343,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B80" t="s">
         <v>18</v>
@@ -2366,11 +2362,15 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81"/>
+      <c r="A81" t="s">
+        <v>10</v>
+      </c>
       <c r="B81" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81"/>
+        <v>18</v>
+      </c>
+      <c r="C81" t="n">
+        <v>5</v>
+      </c>
       <c r="D81" t="n">
         <v>9</v>
       </c>
@@ -2399,13 +2399,13 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B83" t="s">
         <v>18</v>
       </c>
       <c r="C83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D83" t="n">
         <v>10</v>
@@ -2419,13 +2419,13 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
         <v>18</v>
       </c>
       <c r="C84" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D84" t="n">
         <v>10</v>
@@ -2439,13 +2439,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B85" t="s">
         <v>18</v>
       </c>
       <c r="C85" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D85" t="n">
         <v>10</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B86" t="s">
         <v>18</v>
@@ -2479,13 +2479,13 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B87" t="s">
         <v>18</v>
       </c>
       <c r="C87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D87" t="n">
         <v>10</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B93" t="s">
         <v>19</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B94" t="s">
         <v>19</v>
@@ -2627,13 +2627,13 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B95" t="s">
         <v>19</v>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D95" t="n">
         <v>11</v>
@@ -2647,13 +2647,13 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B96" t="s">
         <v>19</v>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D96" t="n">
         <v>11</v>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B97" t="s">
         <v>19</v>
@@ -2687,13 +2687,13 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B98" t="s">
         <v>19</v>
       </c>
       <c r="C98" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D98" t="n">
         <v>11</v>
@@ -2707,13 +2707,13 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B99" t="s">
         <v>19</v>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D99" t="n">
         <v>11</v>
@@ -2743,13 +2743,13 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B101" t="s">
         <v>19</v>
       </c>
       <c r="C101" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D101" t="n">
         <v>12</v>
@@ -2763,13 +2763,13 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B102" t="s">
         <v>19</v>
       </c>
       <c r="C102" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D102" t="n">
         <v>12</v>
@@ -2783,13 +2783,13 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B103" t="s">
         <v>19</v>
       </c>
       <c r="C103" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D103" t="n">
         <v>12</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B104" t="s">
         <v>19</v>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B105" t="s">
         <v>19</v>
@@ -2843,13 +2843,13 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B106" t="s">
         <v>19</v>
       </c>
       <c r="C106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D106" t="n">
         <v>12</v>
@@ -2863,13 +2863,13 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B107" t="s">
         <v>19</v>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D107" t="n">
         <v>12</v>
@@ -2882,11 +2882,15 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108"/>
+      <c r="A108" t="s">
+        <v>8</v>
+      </c>
       <c r="B108" t="s">
-        <v>15</v>
-      </c>
-      <c r="C108"/>
+        <v>19</v>
+      </c>
+      <c r="C108" t="n">
+        <v>2</v>
+      </c>
       <c r="D108" t="n">
         <v>12</v>
       </c>
@@ -2915,13 +2919,13 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B110" t="s">
         <v>19</v>
       </c>
       <c r="C110" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D110" t="n">
         <v>13</v>
@@ -2935,13 +2939,13 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B111" t="s">
         <v>19</v>
       </c>
       <c r="C111" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D111" t="n">
         <v>13</v>
@@ -2955,13 +2959,13 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B112" t="s">
         <v>19</v>
       </c>
       <c r="C112" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D112" t="n">
         <v>13</v>
@@ -2975,13 +2979,13 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B113" t="s">
         <v>19</v>
       </c>
       <c r="C113" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D113" t="n">
         <v>13</v>
@@ -2995,13 +2999,13 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B114" t="s">
         <v>19</v>
       </c>
       <c r="C114" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D114" t="n">
         <v>13</v>
@@ -3015,13 +3019,13 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B115" t="s">
         <v>19</v>
       </c>
       <c r="C115" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D115" t="n">
         <v>13</v>
@@ -3035,13 +3039,13 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B116" t="s">
         <v>19</v>
       </c>
       <c r="C116" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D116" t="n">
         <v>13</v>
@@ -3055,13 +3059,13 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B117" t="s">
         <v>19</v>
       </c>
       <c r="C117" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D117" t="n">
         <v>13</v>
@@ -3091,13 +3095,13 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B119" t="s">
         <v>19</v>
       </c>
       <c r="C119" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D119" t="n">
         <v>14</v>
@@ -3111,13 +3115,13 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B120" t="s">
         <v>19</v>
       </c>
       <c r="C120" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D120" t="n">
         <v>14</v>
@@ -3131,13 +3135,13 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B121" t="s">
         <v>19</v>
       </c>
       <c r="C121" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D121" t="n">
         <v>14</v>
@@ -3151,13 +3155,13 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B122" t="s">
         <v>19</v>
       </c>
       <c r="C122" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D122" t="n">
         <v>14</v>
@@ -3177,7 +3181,7 @@
         <v>19</v>
       </c>
       <c r="C123" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D123" t="n">
         <v>14</v>
@@ -3191,7 +3195,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B124" t="s">
         <v>19</v>
@@ -3211,7 +3215,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B125" t="s">
         <v>19</v>
@@ -3263,13 +3267,13 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B128" t="s">
         <v>19</v>
       </c>
       <c r="C128" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D128" t="n">
         <v>15</v>
@@ -3289,7 +3293,7 @@
         <v>19</v>
       </c>
       <c r="C129" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D129" t="n">
         <v>15</v>
@@ -3303,7 +3307,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B130" t="s">
         <v>19</v>
@@ -3323,13 +3327,13 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B131" t="s">
         <v>19</v>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D131" t="n">
         <v>15</v>
@@ -3343,13 +3347,13 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B132" t="s">
         <v>19</v>
       </c>
       <c r="C132" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D132" t="n">
         <v>15</v>
@@ -3363,7 +3367,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B133" t="s">
         <v>19</v>
@@ -3382,15 +3386,11 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="s">
-        <v>11</v>
-      </c>
+      <c r="A134"/>
       <c r="B134" t="s">
-        <v>19</v>
-      </c>
-      <c r="C134" t="n">
-        <v>4</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C134"/>
       <c r="D134" t="n">
         <v>15</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -3494,10 +3494,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
         <v>98</v>
-      </c>
-      <c r="C4" t="s">
-        <v>99</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -3536,13 +3536,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
         <v>100</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>101</v>
-      </c>
-      <c r="D2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3">
@@ -3550,13 +3550,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>104</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -3766,7 +3766,7 @@
         <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
@@ -3774,10 +3774,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -3816,13 +3816,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3">
@@ -3830,13 +3830,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4">
@@ -3844,10 +3844,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -3886,13 +3886,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3">
@@ -3900,10 +3900,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -3914,10 +3914,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -3956,13 +3956,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -4059,16 +4059,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -4077,19 +4077,19 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
         <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -4109,13 +4109,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
         <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -4127,7 +4127,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -4139,19 +4139,19 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
         <v>0</v>
       </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" t="n">
         <v>1</v>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -4209,10 +4209,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -4224,7 +4224,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -4245,13 +4245,13 @@
         <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -4259,10 +4259,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -4274,7 +4274,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -4292,10 +4292,10 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
         <v>1</v>
@@ -4309,13 +4309,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -4324,10 +4324,10 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
@@ -4336,7 +4336,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
         <v>1</v>
@@ -4359,19 +4359,19 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -4386,19 +4386,19 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
         <v>0</v>
       </c>
-      <c r="K8" t="n">
-        <v>1</v>
-      </c>
       <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" t="n">
         <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N8" t="n">
-        <v>1</v>
       </c>
       <c r="O8" t="n">
         <v>1</v>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -4427,25 +4427,25 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
         <v>0</v>
       </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
         <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>1</v>
       </c>
       <c r="N9" t="n">
         <v>1</v>
@@ -4509,7 +4509,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -4533,28 +4533,28 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
       </c>
       <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P11" t="n">
         <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" t="n">
-        <v>1</v>
-      </c>
-      <c r="P11" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4680,7 +4680,7 @@
         <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -4688,10 +4688,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
         <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -4730,13 +4730,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -4744,13 +4744,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -4820,7 +4820,7 @@
         <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
@@ -4828,10 +4828,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -4870,13 +4870,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">

</xml_diff>